<commit_message>
[New] Config Sheet (config.xlsx)
- Config Sheet 를 추가하였음.
- 여기에 Send 와 Recv 관련 프로토콜을 Title 과 함께, Sheet 명 및 Protocol Size 등을 명시할 계획임.
- 그리고 이 정보를 토대로 프로그램에서는 관련 정보를 Loading 해 올 것임.
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Server\010_Source\Win32\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Client\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582B9080-672E-47BD-A06F-E5506E560718}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344CD1FC-7DA1-442E-A86A-6730537766A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Test" sheetId="3" r:id="rId3"/>
+    <sheet name="Config" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Test" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +67,30 @@
   </si>
   <si>
     <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size (Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send Protocol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recv Protocol</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -238,7 +263,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -282,6 +307,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -610,6 +638,496 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C28626-41F1-4C39-B10D-ED36FC99F958}">
+  <dimension ref="B2:L33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="4.625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="24.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="2.625" customWidth="1"/>
+    <col min="9" max="9" width="4.625" customWidth="1"/>
+    <col min="10" max="11" width="24.625" customWidth="1"/>
+    <col min="12" max="12" width="10.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="I2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="I5" s="5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="I6" s="5">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="5">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="I7" s="5">
+        <v>4</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="I8" s="5">
+        <v>5</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="5">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="I9" s="5">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="I10" s="5">
+        <v>7</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="5">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="I11" s="5">
+        <v>8</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="5">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="I12" s="5">
+        <v>9</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="I13" s="5">
+        <v>10</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="5">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="I14" s="5">
+        <v>11</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="5">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="I15" s="5">
+        <v>12</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="I16" s="5">
+        <v>13</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="I17" s="5">
+        <v>14</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="I18" s="5">
+        <v>15</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="I19" s="5">
+        <v>16</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="I20" s="5">
+        <v>17</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="I21" s="5">
+        <v>18</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="I22" s="5">
+        <v>19</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="I23" s="5">
+        <v>20</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>21</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="I24" s="5">
+        <v>21</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="I25" s="5">
+        <v>22</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="I26" s="5">
+        <v>23</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="5">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="I27" s="5">
+        <v>24</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="5">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="I28" s="5">
+        <v>25</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="5">
+        <v>26</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="I29" s="5">
+        <v>26</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="5">
+        <v>27</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="I30" s="5">
+        <v>27</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="5">
+        <v>28</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="I31" s="5">
+        <v>28</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="5">
+        <v>29</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="I32" s="5">
+        <v>29</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33" s="5">
+        <v>30</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="I33" s="5">
+        <v>30</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="I2:L2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7099D3B-6E8E-476D-873F-90E8792B81C7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -630,11 +1148,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA55F303-B8EC-432B-8E88-A3126BA97215}">
   <dimension ref="C6:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15:K15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Add] Load Protocol List Complete
- Send, Recv Protocol List Load Complete.
- 해당 Sheet 의 실제 존재 여부는 클릭 시 검사하도록 하자.
- 음.. 근데, Sheet 명이 있어야 될 꺼 같은데?
- 일단 커밋.
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Client\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344CD1FC-7DA1-442E-A86A-6730537766A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98DA888-3D8B-49DE-BDC1-735E8D3A18AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
     <sheet name="Config" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
     <sheet name="Test" sheetId="3" r:id="rId4"/>
+    <sheet name="Send_Default" sheetId="5" r:id="rId5"/>
+    <sheet name="Recv_Default" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,6 +93,22 @@
   </si>
   <si>
     <t>Recv Protocol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send_Default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recv_Default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test(Recv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test(Send)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -263,7 +281,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -280,6 +298,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -307,9 +331,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,7 +663,7 @@
   <dimension ref="B2:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -658,18 +679,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="I2" s="15" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="I2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -701,15 +722,27 @@
       <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>32</v>
+      </c>
       <c r="I4" s="5">
         <v>1</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="J4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="2">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
@@ -1328,64 +1361,64 @@
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="8">
         <v>11</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="8">
         <v>22</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="6">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="8">
         <v>33</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="11">
         <v>44</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
@@ -1678,4 +1711,1086 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F342C37-10A9-4F18-8909-0E4D7E93632E}">
+  <dimension ref="C6:L38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.625" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="10.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>7</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="5">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
+        <v>8</v>
+      </c>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="5">
+        <v>8</v>
+      </c>
+      <c r="D15" s="8">
+        <v>11</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="5">
+        <v>9</v>
+      </c>
+      <c r="D16" s="8">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="8">
+        <v>33</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="11">
+        <v>44</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="5">
+        <v>12</v>
+      </c>
+      <c r="D19" s="8">
+        <v>55</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" s="8">
+        <v>66</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8">
+        <v>77</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="5">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="5">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="5">
+        <v>20</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="5">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="5">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="5">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="5">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="5">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="5">
+        <v>26</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="5">
+        <v>27</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="5">
+        <v>28</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="5">
+        <v>29</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="5">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="5">
+        <v>31</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D21:K21"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="D17:K18"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="D20:K20"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FDA293-52BE-4BE6-9EAB-35D8D4577EEB}">
+  <dimension ref="C6:L38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.625" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="10.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>7</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="5">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
+        <v>8</v>
+      </c>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="5">
+        <v>8</v>
+      </c>
+      <c r="D15" s="8">
+        <v>11</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="5">
+        <v>9</v>
+      </c>
+      <c r="D16" s="8">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="8">
+        <v>33</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="11">
+        <v>44</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="5">
+        <v>12</v>
+      </c>
+      <c r="D19" s="11">
+        <v>55</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" s="11">
+        <v>66</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="11">
+        <v>77</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="5">
+        <v>17</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="5">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="5">
+        <v>20</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="5">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="5">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="5">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="5">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="5">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="5">
+        <v>26</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="5">
+        <v>27</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="5">
+        <v>28</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="5">
+        <v>29</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="5">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="5">
+        <v>31</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D23:K24"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="D17:K18"/>
+    <mergeCell ref="D19:K20"/>
+    <mergeCell ref="D21:K22"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Add] 7 Bit Control
- Config Excel File -> Test 를 위한 수정.
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Client\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A78AD-B0BC-499F-8951-F11187CDD69D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C19711-1B05-41A5-B791-E0FD38020D75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
@@ -1718,7 +1718,7 @@
   <dimension ref="C6:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:J29"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2175,28 +2175,36 @@
       <c r="C31" s="5">
         <v>24</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="D31" s="8">
+        <v>71</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="2">
+        <v>72</v>
+      </c>
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C32" s="5">
         <v>25</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="D32" s="2">
+        <v>73</v>
+      </c>
+      <c r="E32" s="8">
+        <v>74</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="10"/>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.3">
@@ -2284,7 +2292,22 @@
       <c r="L38" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="E32:K32"/>
+    <mergeCell ref="D21:K21"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="D17:K18"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="D28:I28"/>
     <mergeCell ref="E29:J29"/>
     <mergeCell ref="F30:K30"/>
@@ -2294,19 +2317,6 @@
     <mergeCell ref="D26:H26"/>
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="J27:K27"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="D21:K21"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="D17:K18"/>
-    <mergeCell ref="D19:K19"/>
-    <mergeCell ref="D20:K20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[New] Globiz Protocol Data Input
- Default Send Protocol & Echo Response Protocol.
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Client\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C19711-1B05-41A5-B791-E0FD38020D75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644C7FE-37C0-4EC5-ACF7-1799D612A009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Test" sheetId="3" r:id="rId4"/>
     <sheet name="Send_Default" sheetId="5" r:id="rId5"/>
     <sheet name="Recv_Default" sheetId="6" r:id="rId6"/>
+    <sheet name="S_Globiz" sheetId="7" r:id="rId7"/>
+    <sheet name="R_Echo_F0" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +111,182 @@
   </si>
   <si>
     <t>Test(Send)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Globiz_Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_Globiz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x47(G)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x42(B)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x31(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x44(D)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character : 'G' (0x47)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character : 'B' (0x42)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character : 'D' (0x44)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character : '1' (0x31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request Sequence Counter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request arg 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Globiz_ECHO_F0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_Echo_F0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Globiz_ECHO_F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_Echo_F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>년</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/100초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>열차번호 문자(ASCII)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000 digit (BCD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 digit (BCD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 digit (BCD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 digit (BCD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Car Number (BCD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1 : Unsigned Char</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2 : Signed Char</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3 : Unsigned Short Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4 : Signed Short Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R5 : Unsigned Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R6 : Signed Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -153,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -275,13 +453,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -298,6 +494,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,6 +530,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -663,7 +871,7 @@
   <dimension ref="B2:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -674,23 +882,23 @@
     <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
     <col min="6" max="8" width="2.625" customWidth="1"/>
     <col min="9" max="9" width="4.625" customWidth="1"/>
-    <col min="10" max="11" width="24.625" customWidth="1"/>
-    <col min="12" max="12" width="10.625" customWidth="1"/>
+    <col min="10" max="11" width="24.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -708,13 +916,13 @@
       <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -748,15 +956,27 @@
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2">
+        <v>20</v>
+      </c>
       <c r="I5" s="5">
         <v>2</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="J5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="2">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
@@ -768,9 +988,15 @@
       <c r="I6" s="5">
         <v>3</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="J6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="2">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
@@ -782,9 +1008,9 @@
       <c r="I7" s="5">
         <v>4</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
@@ -796,9 +1022,9 @@
       <c r="I8" s="5">
         <v>5</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
@@ -810,9 +1036,9 @@
       <c r="I9" s="5">
         <v>6</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
@@ -824,9 +1050,9 @@
       <c r="I10" s="5">
         <v>7</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
@@ -838,9 +1064,9 @@
       <c r="I11" s="5">
         <v>8</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
@@ -852,9 +1078,9 @@
       <c r="I12" s="5">
         <v>9</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
@@ -866,9 +1092,9 @@
       <c r="I13" s="5">
         <v>10</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
@@ -880,9 +1106,9 @@
       <c r="I14" s="5">
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
@@ -894,9 +1120,9 @@
       <c r="I15" s="5">
         <v>12</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
@@ -908,9 +1134,9 @@
       <c r="I16" s="5">
         <v>13</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
@@ -922,9 +1148,9 @@
       <c r="I17" s="5">
         <v>14</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
@@ -936,9 +1162,9 @@
       <c r="I18" s="5">
         <v>15</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
@@ -950,9 +1176,9 @@
       <c r="I19" s="5">
         <v>16</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
@@ -964,9 +1190,9 @@
       <c r="I20" s="5">
         <v>17</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
@@ -978,9 +1204,9 @@
       <c r="I21" s="5">
         <v>18</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
@@ -992,9 +1218,9 @@
       <c r="I22" s="5">
         <v>19</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
@@ -1006,9 +1232,9 @@
       <c r="I23" s="5">
         <v>20</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
@@ -1020,9 +1246,9 @@
       <c r="I24" s="5">
         <v>21</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
@@ -1034,9 +1260,9 @@
       <c r="I25" s="5">
         <v>22</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
@@ -1048,9 +1274,9 @@
       <c r="I26" s="5">
         <v>23</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
@@ -1062,9 +1288,9 @@
       <c r="I27" s="5">
         <v>24</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
@@ -1076,9 +1302,9 @@
       <c r="I28" s="5">
         <v>25</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
@@ -1090,9 +1316,9 @@
       <c r="I29" s="5">
         <v>26</v>
       </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="5">
@@ -1104,9 +1330,9 @@
       <c r="I30" s="5">
         <v>27</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="5">
@@ -1118,9 +1344,9 @@
       <c r="I31" s="5">
         <v>28</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="5">
@@ -1132,9 +1358,9 @@
       <c r="I32" s="5">
         <v>29</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="5">
@@ -1146,9 +1372,9 @@
       <c r="I33" s="5">
         <v>30</v>
       </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1361,64 +1587,64 @@
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <v>11</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <v>22</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="8">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="9">
         <v>33</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="12">
         <v>44</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
@@ -1717,7 +1943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F342C37-10A9-4F18-8909-0E4D7E93632E}">
   <dimension ref="C6:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -1893,150 +2119,150 @@
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <v>11</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <v>22</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="8">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="9">
         <v>33</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="12">
         <v>44</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="9">
         <v>55</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>13</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="9">
         <v>66</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>14</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="9">
         <v>77</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>15</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <v>151</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="8">
+      <c r="E22" s="11"/>
+      <c r="F22" s="9">
         <v>152</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="8">
+      <c r="G22" s="11"/>
+      <c r="H22" s="9">
         <v>153</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="8">
+      <c r="I22" s="11"/>
+      <c r="J22" s="9">
         <v>154</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>16</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="9">
         <v>161</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="8">
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="9">
         <v>162</v>
       </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="2">
         <v>163</v>
       </c>
@@ -2052,31 +2278,31 @@
       <c r="D24" s="2">
         <v>171</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="9">
         <v>172</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="2">
         <v>173</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="9">
         <v>174</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" s="5">
         <v>18</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="9">
         <v>181</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="2">
         <v>182</v>
       </c>
@@ -2095,13 +2321,13 @@
       <c r="C26" s="5">
         <v>19</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="9">
         <v>191</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -2112,29 +2338,29 @@
         <v>20</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="8">
+      <c r="E27" s="9">
         <v>201</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="11"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" s="5">
         <v>21</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="9">
         <v>211</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="11"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="3"/>
@@ -2144,14 +2370,14 @@
         <v>22</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="8">
+      <c r="E29" s="9">
         <v>221</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="11"/>
       <c r="K29" s="2"/>
       <c r="L29" s="3"/>
     </row>
@@ -2161,29 +2387,29 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="8">
+      <c r="F30" s="9">
         <v>231</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C31" s="5">
         <v>24</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="9">
         <v>71</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="11"/>
       <c r="K31" s="2">
         <v>72</v>
       </c>
@@ -2196,15 +2422,15 @@
       <c r="D32" s="2">
         <v>73</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="9">
         <v>74</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="11"/>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.3">
@@ -2293,6 +2519,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="J27:K27"/>
     <mergeCell ref="D31:J31"/>
     <mergeCell ref="E32:K32"/>
     <mergeCell ref="D21:K21"/>
@@ -2309,14 +2543,6 @@
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="D28:I28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="J27:K27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2503,154 +2729,154 @@
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <v>11</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <v>22</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="8">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="9">
         <v>33</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="12">
         <v>44</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="12">
         <v>55</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>13</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>14</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="12">
         <v>66</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>15</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>16</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="12">
         <v>77</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="14"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>17</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="16"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
@@ -2862,4 +3088,1014 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ADA6599-698C-466C-BA1E-0C2E1E77F54E}">
+  <dimension ref="C6:L26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.625" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="10.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.75" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="5">
+        <v>7</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="5">
+        <v>8</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="5">
+        <v>9</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="5">
+        <v>12</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="5">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="5">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="D14:K14"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="D20:K20"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3E9680-8588-4D1A-BEAF-5E71804376D3}">
+  <dimension ref="C6:L40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.625" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="10.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.75" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="5">
+        <v>7</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="5">
+        <v>8</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="5">
+        <v>9</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="5">
+        <v>12</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="5">
+        <v>17</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>18</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="5">
+        <v>19</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="5">
+        <v>20</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="5">
+        <v>21</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="5">
+        <v>22</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="5">
+        <v>23</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="5">
+        <v>24</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="5">
+        <v>25</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="5">
+        <v>26</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="5">
+        <v>27</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="5">
+        <v>28</v>
+      </c>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="5">
+        <v>29</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="5">
+        <v>30</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="5">
+        <v>31</v>
+      </c>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="5">
+        <v>32</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C40" s="5">
+        <v>33</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="D31:K32"/>
+    <mergeCell ref="D33:K36"/>
+    <mergeCell ref="D37:K40"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="D29:K30"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="D21:K21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="D14:K14"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="D12:K12"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Mod] Config.xlsx (Del Sheet)
- Test Sheet 추가 삭제.
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Client\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9BF3A4-3C68-4D8C-8B0D-0BE85E939D23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082647F9-AA24-4B56-B635-347720BB11AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="791" activeTab="2" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
     <sheet name="Config" sheetId="4" r:id="rId2"/>
-    <sheet name="Test" sheetId="3" r:id="rId3"/>
-    <sheet name="Send_Default" sheetId="5" r:id="rId4"/>
-    <sheet name="Recv_Default" sheetId="6" r:id="rId5"/>
-    <sheet name="S_Globiz" sheetId="7" r:id="rId6"/>
-    <sheet name="S_F0" sheetId="10" r:id="rId7"/>
-    <sheet name="R_F0" sheetId="9" r:id="rId8"/>
+    <sheet name="Send_Default" sheetId="5" r:id="rId3"/>
+    <sheet name="Recv_Default" sheetId="6" r:id="rId4"/>
+    <sheet name="S_Globiz" sheetId="7" r:id="rId5"/>
+    <sheet name="S_F0" sheetId="10" r:id="rId6"/>
+    <sheet name="R_F0" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -901,7 +900,7 @@
   <dimension ref="B2:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1417,543 +1416,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA55F303-B8EC-432B-8E88-A3126BA97215}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F342C37-10A9-4F18-8909-0E4D7E93632E}">
   <dimension ref="C6:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="2.625" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
-    <col min="4" max="11" width="10.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="23.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="6" spans="3:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="5">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
-        <v>3</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="5">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="5">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2">
-        <v>5</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="5">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <v>6</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="5">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2">
-        <v>7</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="5">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2">
-        <v>8</v>
-      </c>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="5">
-        <v>8</v>
-      </c>
-      <c r="D15" s="10">
-        <v>11</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="5">
-        <v>9</v>
-      </c>
-      <c r="D16" s="10">
-        <v>22</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="10">
-        <v>33</v>
-      </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="5">
-        <v>10</v>
-      </c>
-      <c r="D17" s="13">
-        <v>44</v>
-      </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C18" s="5">
-        <v>11</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="5">
-        <v>12</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="5">
-        <v>13</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21" s="5">
-        <v>14</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="5">
-        <v>15</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="5">
-        <v>16</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="5">
-        <v>17</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="5">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C26" s="5">
-        <v>19</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C27" s="5">
-        <v>20</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C28" s="5">
-        <v>21</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="5">
-        <v>22</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="5">
-        <v>23</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C31" s="5">
-        <v>24</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C32" s="5">
-        <v>25</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C33" s="5">
-        <v>26</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="5">
-        <v>27</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C35" s="5">
-        <v>28</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C36" s="5">
-        <v>29</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="5">
-        <v>30</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C38" s="5">
-        <v>31</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="D17:K18"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F342C37-10A9-4F18-8909-0E4D7E93632E}">
-  <dimension ref="C6:L38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2528,14 +1995,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="J27:K27"/>
     <mergeCell ref="D31:J31"/>
     <mergeCell ref="E32:K32"/>
     <mergeCell ref="D21:K21"/>
@@ -2552,13 +2011,21 @@
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="D28:I28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="J27:K27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FDA293-52BE-4BE6-9EAB-35D8D4577EEB}">
   <dimension ref="C6:L38"/>
   <sheetViews>
@@ -3099,7 +2566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ADA6599-698C-466C-BA1E-0C2E1E77F54E}">
   <dimension ref="C6:L26"/>
   <sheetViews>
@@ -3485,7 +2952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66354DE2-1688-4D2C-BE31-CB8D784B1363}">
   <dimension ref="C6:L26"/>
   <sheetViews>
@@ -3847,25 +3314,25 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D23:K26"/>
+    <mergeCell ref="D15:K16"/>
+    <mergeCell ref="D17:K18"/>
+    <mergeCell ref="D19:K22"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="D14:K14"/>
     <mergeCell ref="D12:K12"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="D8:K8"/>
     <mergeCell ref="D9:K9"/>
     <mergeCell ref="D10:K10"/>
     <mergeCell ref="D11:K11"/>
-    <mergeCell ref="D23:K26"/>
-    <mergeCell ref="D15:K16"/>
-    <mergeCell ref="D17:K18"/>
-    <mergeCell ref="D19:K22"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="D14:K14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3E9680-8588-4D1A-BEAF-5E71804376D3}">
   <dimension ref="C6:L40"/>
   <sheetViews>
@@ -4455,15 +3922,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D31:K32"/>
-    <mergeCell ref="D33:K36"/>
-    <mergeCell ref="D37:K40"/>
-    <mergeCell ref="D24:K24"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="D29:K30"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="D11:K11"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="D23:G23"/>
     <mergeCell ref="D13:K13"/>
@@ -4477,12 +3941,15 @@
     <mergeCell ref="D21:K21"/>
     <mergeCell ref="D22:G22"/>
     <mergeCell ref="H22:K22"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="D9:K9"/>
-    <mergeCell ref="D10:K10"/>
-    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="D31:K32"/>
+    <mergeCell ref="D33:K36"/>
+    <mergeCell ref="D37:K40"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="D29:K30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Mod] Config.xlsx (Change Sheet Name)
- Test Sheet 를 하나만 두었음. 기존 Test Sheet Name 을 이로 변경.
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Client\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082647F9-AA24-4B56-B635-347720BB11AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B0CD99-D241-4E94-8C33-98CA44BE33E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="791" activeTab="2" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="791" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
     <sheet name="Config" sheetId="4" r:id="rId2"/>
-    <sheet name="Send_Default" sheetId="5" r:id="rId3"/>
+    <sheet name="Test" sheetId="5" r:id="rId3"/>
     <sheet name="Recv_Default" sheetId="6" r:id="rId4"/>
     <sheet name="S_Globiz" sheetId="7" r:id="rId5"/>
     <sheet name="S_F0" sheetId="10" r:id="rId6"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t>Byte</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,14 +97,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Send_Default</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recv_Default</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test(Recv)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -310,6 +302,10 @@
   </si>
   <si>
     <t>R_F0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -500,7 +496,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -526,6 +522,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -899,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C28626-41F1-4C39-B10D-ED36FC99F958}">
   <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -916,18 +915,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -960,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="E4" s="2">
         <v>32</v>
@@ -972,10 +971,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="L4" s="2">
         <v>32</v>
@@ -986,10 +985,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
         <v>20</v>
@@ -998,10 +997,10 @@
         <v>2</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L5" s="2">
         <v>34</v>
@@ -1012,10 +1011,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2">
         <v>20</v>
@@ -1419,7 +1418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F342C37-10A9-4F18-8909-0E4D7E93632E}">
   <dimension ref="C6:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
@@ -1595,150 +1594,150 @@
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="11">
         <v>11</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
         <v>22</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="10">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="11">
         <v>33</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="14">
         <v>44</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="16"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="19"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="11">
         <v>55</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>13</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="11">
         <v>66</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>14</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="11">
         <v>77</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>15</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="11">
         <v>151</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="10">
+      <c r="E22" s="13"/>
+      <c r="F22" s="11">
         <v>152</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="10">
+      <c r="G22" s="13"/>
+      <c r="H22" s="11">
         <v>153</v>
       </c>
-      <c r="I22" s="12"/>
-      <c r="J22" s="10">
+      <c r="I22" s="13"/>
+      <c r="J22" s="11">
         <v>154</v>
       </c>
-      <c r="K22" s="12"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>16</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="11">
         <v>161</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="10">
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="11">
         <v>162</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="2">
         <v>163</v>
       </c>
@@ -1754,31 +1753,31 @@
       <c r="D24" s="2">
         <v>171</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="11">
         <v>172</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="2">
         <v>173</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="11">
         <v>174</v>
       </c>
-      <c r="J24" s="11"/>
-      <c r="K24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" s="5">
         <v>18</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="11">
         <v>181</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="2">
         <v>182</v>
       </c>
@@ -1797,13 +1796,13 @@
       <c r="C26" s="5">
         <v>19</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="11">
         <v>191</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1814,29 +1813,29 @@
         <v>20</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="10">
+      <c r="E27" s="11">
         <v>201</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" s="5">
         <v>21</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="11">
         <v>211</v>
       </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="3"/>
@@ -1846,14 +1845,14 @@
         <v>22</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="10">
+      <c r="E29" s="11">
         <v>221</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="2"/>
       <c r="L29" s="3"/>
     </row>
@@ -1863,29 +1862,29 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="10">
+      <c r="F30" s="11">
         <v>231</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C31" s="5">
         <v>24</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="11">
         <v>71</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
       <c r="K31" s="2">
         <v>72</v>
       </c>
@@ -1898,15 +1897,15 @@
       <c r="D32" s="2">
         <v>73</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="11">
         <v>74</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="13"/>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.3">
@@ -1995,6 +1994,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="J27:K27"/>
     <mergeCell ref="D31:J31"/>
     <mergeCell ref="E32:K32"/>
     <mergeCell ref="D21:K21"/>
@@ -2011,14 +2018,6 @@
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="D28:I28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="J27:K27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2205,154 +2204,154 @@
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="11">
         <v>11</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
         <v>22</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="10">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="11">
         <v>33</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="14">
         <v>44</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="16"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="19"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="14">
         <v>55</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>13</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="19"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>14</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="14">
         <v>66</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>15</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>16</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="14">
         <v>77</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>17</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="19"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
@@ -2618,232 +2617,232 @@
       <c r="C7" s="5">
         <v>0</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
+      <c r="D7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
+      <c r="D8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
       <c r="L10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>4</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>5</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
+      <c r="D12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>6</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
+      <c r="D13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>7</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
+      <c r="D14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
+      <c r="D15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
+      <c r="D16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="12"/>
+      <c r="D17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
+      <c r="D18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="13"/>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
+      <c r="D19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>13</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="12"/>
+      <c r="D20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
@@ -3004,328 +3003,328 @@
       <c r="C7" s="5">
         <v>0</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
+      <c r="D7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
+      <c r="D8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
       <c r="L10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>4</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>5</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
+      <c r="D12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>6</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
+      <c r="D13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>7</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
+      <c r="D14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="D15" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="D17" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="D19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>13</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>14</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>15</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>16</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="D23" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>17</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" s="5">
         <v>18</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26" s="5">
         <v>19</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="D11:K11"/>
     <mergeCell ref="D23:K26"/>
     <mergeCell ref="D15:K16"/>
     <mergeCell ref="D17:K18"/>
     <mergeCell ref="D19:K22"/>
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="D9:K9"/>
-    <mergeCell ref="D10:K10"/>
-    <mergeCell ref="D11:K11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3384,550 +3383,553 @@
       <c r="C7" s="5">
         <v>0</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
+      <c r="D7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
+      <c r="D8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
       <c r="L10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>4</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>5</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
+      <c r="D12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>6</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
+      <c r="D13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>7</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
+      <c r="D14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C15" s="5">
         <v>8</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
+      <c r="D15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C16" s="5">
         <v>9</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
+      <c r="D16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="12"/>
+      <c r="D17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5">
         <v>11</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
+      <c r="D18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="13"/>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
+      <c r="D19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>13</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="12"/>
+      <c r="D20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>14</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="12"/>
+      <c r="D21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>15</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="12"/>
+      <c r="D22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>16</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="12"/>
+      <c r="D23" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>17</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="12"/>
+      <c r="D24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" s="5">
         <v>18</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="12"/>
+      <c r="D25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26" s="5">
         <v>19</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="12"/>
+      <c r="D26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" s="5">
         <v>20</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="12"/>
+      <c r="D27" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" s="5">
         <v>21</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="12"/>
+      <c r="D28" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C29" s="5">
         <v>22</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
+      <c r="D29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="16"/>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C30" s="5">
         <v>23</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="19"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C31" s="5">
         <v>24</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="15"/>
+      <c r="D31" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="16"/>
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C32" s="5">
         <v>25</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="18"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19"/>
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C33" s="5">
         <v>26</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="15"/>
+      <c r="D33" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="16"/>
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C34" s="5">
         <v>27</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="22"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="23"/>
       <c r="L34" s="2"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C35" s="5">
         <v>28</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="22"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="23"/>
       <c r="L35" s="2"/>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C36" s="5">
         <v>29</v>
       </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="18"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="19"/>
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C37" s="5">
         <v>30</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="15"/>
+      <c r="D37" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="16"/>
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C38" s="5">
         <v>31</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="22"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="23"/>
       <c r="L38" s="2"/>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C39" s="5">
         <v>32</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="22"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="23"/>
       <c r="L39" s="2"/>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C40" s="5">
         <v>33</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="18"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="19"/>
       <c r="L40" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="D9:K9"/>
-    <mergeCell ref="D10:K10"/>
-    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="D31:K32"/>
+    <mergeCell ref="D33:K36"/>
+    <mergeCell ref="D37:K40"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="D29:K30"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="D23:G23"/>
     <mergeCell ref="D13:K13"/>
@@ -3941,15 +3943,12 @@
     <mergeCell ref="D21:K21"/>
     <mergeCell ref="D22:G22"/>
     <mergeCell ref="H22:K22"/>
-    <mergeCell ref="D31:K32"/>
-    <mergeCell ref="D33:K36"/>
-    <mergeCell ref="D37:K40"/>
-    <mergeCell ref="D24:K24"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="D29:K30"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="D11:K11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>